<commit_message>
A2A_D2D_INT Booking done 19th mar
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/A2A_Booking.xlsx
+++ b/src/main/java/com/crm/qa/testdata/A2A_Booking.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455" tabRatio="918" firstSheet="20" activeTab="22"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455" tabRatio="918" firstSheet="16" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="A2A_PrePaid_A2A TC3" sheetId="1" r:id="rId1"/>
@@ -1985,8 +1985,8 @@
   </sheetPr>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2780,7 +2780,7 @@
   </sheetPr>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>

</xml_diff>